<commit_message>
Did the bulk of the work on our experimental materials, time to modify our old qualtrics survey and then get to it!
</commit_message>
<xml_diff>
--- a/Medical Yearly Costs/CHAT prototype/Medical Cost Descriptions PLAIN.xlsx
+++ b/Medical Yearly Costs/CHAT prototype/Medical Cost Descriptions PLAIN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Grad School\2022-2023\psych-phd\Medical Yearly Costs\CHAT prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5F6AB8-CF1A-4B97-BC9B-6DDC235A7955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B8AD4C-4FE3-436B-90F3-265418C53601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13920" yWindow="11508" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Primary</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>Advanced</t>
-  </si>
-  <si>
-    <t>originally 47/72</t>
-  </si>
-  <si>
-    <t>70 total.. Try 45/46?</t>
   </si>
   <si>
     <t>1 point: Covers “alternative” services including acupuncture (for pain), spiritual healing or Reiki, and therapeutic massage.</t>
@@ -520,156 +514,103 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">2 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>You get minimal dental care.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 + 4 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>You get complete dental care including repairs and crowns.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Your insurance pays in full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> for up to: 2 weekly visits from a nurse OR 2, 1/2 hr daily care from a nurse's aide.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2 + 1 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Your insurance pays in full</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> for up to: 4 weekly visits from a nurse OR 5 hr daily care from a nurse's aide.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>7 points:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You need your primary doctor's referral to see a specialist in your plan.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You wait about 45 days for an appointment. There are few specialties available.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You pay $10 a visit. If you visit a specialist outside of your plan you pay for it yourself.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">7 + 7 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>You may see a specialist without a referral from your primary doctor.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You wait only a few days for an appointment. There are many specialties available. You may go to almost any specialist in your area. </t>
+      <t xml:space="preserve">1+ 1 points: There is no review process. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Your health plan pays in full for any and all equipment.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 point: Your health insurance company reviews your need first. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Your health plan decides if it will pay for all, some, or none of the equipment requested.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 point: You get an eye exam every 2 years. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>You pay $5 per visit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 + 1 point: You get an eye exam every 2 years. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>You pay $5 per visit. You receive $75 for lenses and frames if needed every 2 years.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cost Burden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 points: You get minimal dental care. You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 + 4 points: You get complete dental care including repairs and crowns. You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. </t>
+  </si>
+  <si>
+    <t>2 + 1 points: Your insurance pays in full for up to: 4 weekly visits from a nurse OR 5 hr daily care from a nurse's aide.</t>
+  </si>
+  <si>
+    <t>2 points: Your insurance pays in full for up to: 2 weekly visits from a nurse OR 2, 1/2 hr daily care from a nurse's aide.</t>
+  </si>
+  <si>
+    <t>3 points: Your doctor needs to get expensive tests approved before ordering them. You might need the test done at a lab far away from your doctor's office.</t>
+  </si>
+  <si>
+    <t>3 + 1 points: Your doctor can order any tests for you without getting approval. You can have the tests done at or near your doctor's office.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7 points: You need your primary doctor's referral to see a specialist in your plan. You wait about 45 days for an appointment. There are few specialties available. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>You pay $10 a visit. If you visit a specialist outside of your plan you pay for it yourself.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7 + 7 points: You may see a specialist without a referral from your primary doctor. You wait only a few days for an appointment. There are many specialties available. You may go to almost any specialist in your area. </t>
     </r>
     <r>
       <rPr>
@@ -683,137 +624,830 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1+ 1 points: There is no review process. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Your health plan pays in full for any and all equipment.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1 point: Your health insurance company reviews your need first. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Your health plan decides if it will pay for all, some, or none of the equipment requested.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1 point: You get an eye exam every 2 years. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>You pay $5 per visit.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1 + 1 point: You get an eye exam every 2 years. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>You pay $5 per visit. You receive $75 for lenses and frames if needed every 2 years.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Your doctor needs to get expensive tests approved before ordering them.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You might need the test done at a lab far away from your doctor's office.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">3 + 1 points: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Your doctor can order any tests for you without getting approval.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> You can have the tests done at or near your doctor's office.</t>
-    </r>
-  </si>
-  <si>
-    <t>Average spent per person per year thru PHI: $4740.5</t>
-  </si>
-  <si>
-    <t>Average spent per person per year thru GHI: $11,467.8</t>
-  </si>
-  <si>
-    <t>Cost Burden</t>
-  </si>
-  <si>
-    <t>Yearly spent by private health insurance = 1,000,234 for 211</t>
-  </si>
-  <si>
-    <t>Total personal health care (total that should be spent outside of investment/administrative fees) in mil = 3357832 for 329</t>
-  </si>
-  <si>
-    <t>Yearly spent by Govt health insurance = 1,490,818 for 106?</t>
+    <t>Total Spending</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$98.63</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$1938.28</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$3397.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$180.58</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$1424.85</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$1334.82</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$141.21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$667.71</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> $531.48</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$137.62</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> $79.23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$818.95</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Out of Pocket:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> $180.58</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> $1424.85</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$1334.82</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$161.70</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$282.97</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$194.41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$38.36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$74.38</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$618.26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$1181.30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$4740.45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$9029.45</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$78.33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$155.85</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$127.66</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$70.73</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$50.16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$131.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$172.99</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Out of Pocket: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$128.62</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Private Insurance: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$25.98</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year
+Medicaid: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$120.46</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / Year</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -875,13 +1509,50 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -913,9 +1584,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -931,11 +1599,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1278,225 +1947,251 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.88671875" customWidth="1"/>
     <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
     <col min="6" max="6" width="19.77734375" customWidth="1"/>
     <col min="7" max="7" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="124.2" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>57</v>
+    <row r="13" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="92.4" x14ac:dyDescent="0.5">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="102.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="55.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="51.6" x14ac:dyDescent="0.5">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="6" t="s">
+    <row r="14" spans="1:5" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>52</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>